<commit_message>
update login credentials data file
</commit_message>
<xml_diff>
--- a/Data Files/Login Credentials.xlsx
+++ b/Data Files/Login Credentials.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
   <si>
     <t>https://sandbox.vsms.tezzasolutions.com/index</t>
   </si>
@@ -52,12 +52,15 @@
   </si>
   <si>
     <t>dennis.gituto@tezzasolutions.com</t>
+  </si>
+  <si>
+    <t>!qwerty123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -110,6 +113,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -157,7 +163,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -190,9 +196,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -225,6 +248,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -400,21 +440,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" activeCellId="1" sqref="B1 C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="44.7109375" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="1" max="1" width="44.7265625" customWidth="1"/>
+    <col min="2" max="2" width="31.453125" customWidth="1"/>
+    <col min="3" max="3" width="26.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -425,7 +465,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -436,36 +476,36 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2"/>
-    <hyperlink ref="A2" r:id="rId3"/>
-    <hyperlink ref="A3" r:id="rId4"/>
-    <hyperlink ref="B2" r:id="rId5"/>
-    <hyperlink ref="B3" r:id="rId6"/>
+    <hyperlink ref="A4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B3" r:id="rId5" xr:uid="{0CA975AD-8A5C-42FA-ACC4-DEA53D50A808}"/>
+    <hyperlink ref="B4" r:id="rId6" xr:uid="{B4EBD021-41A2-49EB-9195-CD2D282BFFDA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId7"/>
@@ -473,20 +513,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35.5703125" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="35.54296875" customWidth="1"/>
+    <col min="2" max="2" width="18.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -494,7 +534,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -502,7 +542,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -512,29 +552,29 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" customWidth="1"/>
-    <col min="2" max="2" width="32.28515625" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" customWidth="1"/>
+    <col min="1" max="1" width="21.54296875" customWidth="1"/>
+    <col min="2" max="2" width="32.26953125" customWidth="1"/>
+    <col min="3" max="3" width="21.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -547,8 +587,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1"/>
-    <hyperlink ref="B1" r:id="rId2"/>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="B1" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>